<commit_message>
updata scrollupdowntillelement this method
</commit_message>
<xml_diff>
--- a/DataSheet/CPC_Dynamic.xlsx
+++ b/DataSheet/CPC_Dynamic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BSA_MOBILE_FRAMEWORK\DataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B82109-8A36-4880-A3CB-66F8A8274ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8365A7-B379-4FC1-BB12-0B6E896365D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{875AE543-1650-41B3-9C38-4B818EB686AA}"/>
   </bookViews>
@@ -851,7 +851,7 @@
     <t>ScrollDown(1400)</t>
   </si>
   <si>
-    <t>MF24121100006530</t>
+    <t>MF24121200005873</t>
   </si>
 </sst>
 </file>
@@ -15114,7 +15114,7 @@
     </row>
     <row r="518" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A518" s="2">
-        <f t="shared" ref="A518:A527" si="59">A516+1</f>
+        <f t="shared" ref="A518:A526" si="59">A516+1</f>
         <v>1</v>
       </c>
       <c r="B518" t="s">
@@ -16318,7 +16318,7 @@
   <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added coapplicant excle sheet
</commit_message>
<xml_diff>
--- a/DataSheet/CPC_Dynamic.xlsx
+++ b/DataSheet/CPC_Dynamic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BSA_MOBILE_FRAMEWORK\DataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8365A7-B379-4FC1-BB12-0B6E896365D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F86469-672D-4548-9442-4F6D086212B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{875AE543-1650-41B3-9C38-4B818EB686AA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{875AE543-1650-41B3-9C38-4B818EB686AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4320" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4330" uniqueCount="229">
   <si>
     <t>Si_No</t>
   </si>
@@ -851,7 +851,13 @@
     <t>ScrollDown(1400)</t>
   </si>
   <si>
-    <t>MF24121200005873</t>
+    <t>ScrollDown(1300)</t>
+  </si>
+  <si>
+    <t>QUIT</t>
+  </si>
+  <si>
+    <t>MF24121300006016</t>
   </si>
 </sst>
 </file>
@@ -1279,10 +1285,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC0CA32F-6895-4985-AF4D-119BC41D4938}">
-  <dimension ref="A1:O561"/>
+  <dimension ref="A1:O562"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="77" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="A543" zoomScale="77" workbookViewId="0">
+      <selection activeCell="H563" sqref="H563"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11319,7 +11325,7 @@
       </c>
       <c r="F364" s="1"/>
       <c r="H364" s="1" t="s">
-        <v>101</v>
+        <v>226</v>
       </c>
       <c r="J364" t="s">
         <v>16</v>
@@ -16305,6 +16311,41 @@
       </c>
       <c r="O561" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="562" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A562" s="2">
+        <v>2</v>
+      </c>
+      <c r="B562" t="s">
+        <v>81</v>
+      </c>
+      <c r="C562" t="s">
+        <v>17</v>
+      </c>
+      <c r="D562" t="s">
+        <v>15</v>
+      </c>
+      <c r="H562" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="J562" t="s">
+        <v>16</v>
+      </c>
+      <c r="K562" t="s">
+        <v>43</v>
+      </c>
+      <c r="L562" t="s">
+        <v>18</v>
+      </c>
+      <c r="M562" t="s">
+        <v>45</v>
+      </c>
+      <c r="N562" t="s">
+        <v>34</v>
+      </c>
+      <c r="O562" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -16317,8 +16358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A86AEA-BDCA-4ACF-93E7-52FBBDAF5EE7}">
   <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16485,7 +16526,7 @@
         <v>78</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>84</v>

</xml_diff>